<commit_message>
Created new split table
Split table into three historical periods
</commit_message>
<xml_diff>
--- a/Lit_Review_Tables.xlsx
+++ b/Lit_Review_Tables.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7350"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7350" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Split Tables" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>Method</t>
   </si>
@@ -163,13 +164,64 @@
   </si>
   <si>
     <t>Non-linear</t>
+  </si>
+  <si>
+    <t>Group 1: Historical Performance Management Methods</t>
+  </si>
+  <si>
+    <t>Failure Analysis</t>
+  </si>
+  <si>
+    <t>FMEA / FMECA</t>
+  </si>
+  <si>
+    <t>Fault Tree Analysis</t>
+  </si>
+  <si>
+    <t>Group 2: Real-time performance management methods</t>
+  </si>
+  <si>
+    <t>Performance Analysis</t>
+  </si>
+  <si>
+    <t>Mathematical simulation</t>
+  </si>
+  <si>
+    <t>Engineering rules</t>
+  </si>
+  <si>
+    <t>Reactive controls</t>
+  </si>
+  <si>
+    <t>Group 3: Predictive performance management methods</t>
+  </si>
+  <si>
+    <t>Automatic performance analysis</t>
+  </si>
+  <si>
+    <t>Statistical Learning</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Examples</t>
+  </si>
+  <si>
+    <t>Capabilities</t>
+  </si>
+  <si>
+    <t>Methods</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +257,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -226,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -408,11 +469,224 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -427,15 +701,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -458,6 +723,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,7 +1081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -827,25 +1116,25 @@
       </c>
     </row>
     <row r="3" spans="3:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="24"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="3:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="C4" s="15"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="18" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="1"/>
@@ -853,37 +1142,37 @@
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="3:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="C5" s="15"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="19" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="11"/>
-      <c r="J5" s="23"/>
+      <c r="J5" s="20"/>
     </row>
     <row r="6" spans="3:12" ht="45.75" x14ac:dyDescent="0.3">
-      <c r="C6" s="15"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="18" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="9"/>
-      <c r="L6" s="18"/>
+      <c r="L6" s="15"/>
     </row>
     <row r="7" spans="3:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="C7" s="15"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="19" t="s">
         <v>27</v>
       </c>
       <c r="F7" s="10"/>
@@ -893,24 +1182,24 @@
       </c>
     </row>
     <row r="8" spans="3:12" ht="90.75" x14ac:dyDescent="0.3">
-      <c r="C8" s="15"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="18" t="s">
         <v>28</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="9"/>
-      <c r="J8" s="19"/>
+      <c r="J8" s="16"/>
     </row>
     <row r="9" spans="3:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="C9" s="15"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="18" t="s">
         <v>34</v>
       </c>
       <c r="F9" s="1"/>
@@ -918,22 +1207,22 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="3:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="C10" s="15"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="19" t="s">
         <v>31</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="11"/>
     </row>
     <row r="11" spans="3:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="C11" s="16"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="18" t="s">
         <v>32</v>
       </c>
       <c r="F11" s="1"/>
@@ -1237,4 +1526,277 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="26"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="27"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="27"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="26"/>
+      <c r="C6" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="27"/>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="26"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="27"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="27"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="26"/>
+      <c r="C11" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="27"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="26"/>
+      <c r="C12" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="27"/>
+    </row>
+    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="30"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="39"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="26"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="27"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="27"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="26"/>
+      <c r="C17" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="27"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
+      <c r="C18" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="27"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="26"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="27"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="26"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="27"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="26"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="27"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="26"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="27"/>
+    </row>
+    <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="30"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="34"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="36"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="26"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="27"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="26"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="27"/>
+    </row>
+    <row r="27" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="28"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added to model-based section
Took reference from gertler book
</commit_message>
<xml_diff>
--- a/Lit_Review_Tables.xlsx
+++ b/Lit_Review_Tables.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Method</t>
   </si>
@@ -247,6 +247,9 @@
   <si>
     <t>Large time commitment required for each and every implementation
 Difficult to transfer lessons learned to new applicatinos</t>
+  </si>
+  <si>
+    <t>Kalman Filter</t>
   </si>
 </sst>
 </file>
@@ -716,48 +719,69 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -770,26 +794,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -799,12 +808,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1175,7 +1178,7 @@
       </c>
     </row>
     <row r="3" spans="3:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="38" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="14" t="s">
@@ -1189,7 +1192,7 @@
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="3:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="C4" s="23"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1201,7 +1204,7 @@
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="3:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="C5" s="23"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="10" t="s">
         <v>14</v>
       </c>
@@ -1214,7 +1217,7 @@
       <c r="J5" s="20"/>
     </row>
     <row r="6" spans="3:12" ht="45.75" x14ac:dyDescent="0.3">
-      <c r="C6" s="23"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1227,7 +1230,7 @@
       <c r="L6" s="15"/>
     </row>
     <row r="7" spans="3:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="C7" s="23"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
@@ -1241,7 +1244,7 @@
       </c>
     </row>
     <row r="8" spans="3:12" ht="90.75" x14ac:dyDescent="0.3">
-      <c r="C8" s="23"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1254,7 +1257,7 @@
       <c r="J8" s="16"/>
     </row>
     <row r="9" spans="3:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="C9" s="23"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1266,7 +1269,7 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="3:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="C10" s="23"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="10" t="s">
         <v>30</v>
       </c>
@@ -1277,7 +1280,7 @@
       <c r="H10" s="11"/>
     </row>
     <row r="11" spans="3:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="C11" s="24"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1592,315 +1595,317 @@
   <dimension ref="B1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="25"/>
-    <col min="2" max="2" width="16.140625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" style="25" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" style="25" customWidth="1"/>
-    <col min="7" max="8" width="21.140625" style="25" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="25"/>
+    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="2" max="2" width="16.140625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="25" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" style="22" customWidth="1"/>
+    <col min="7" max="8" width="21.140625" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="25" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="48" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="30" t="s">
+      <c r="E3" s="26"/>
+      <c r="F3" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="53" t="s">
+      <c r="H3" s="55" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="44"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="49" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="54"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="56"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="44"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="50" t="s">
+      <c r="B5" s="51"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="54"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="56"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="44"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="50" t="s">
+      <c r="B6" s="51"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="54"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="56"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="44"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="50" t="s">
+      <c r="B7" s="51"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="54"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="56"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="44"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="51" t="s">
+      <c r="B8" s="51"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="54"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="56"/>
     </row>
     <row r="9" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B9" s="44"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="51" t="s">
+      <c r="B9" s="51"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="54"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="56"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="44"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="51" t="s">
+      <c r="B10" s="51"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="54"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="56"/>
     </row>
     <row r="11" spans="2:8" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="45"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="52" t="s">
+      <c r="B11" s="52"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="55"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="57"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30" t="s">
+      <c r="C12" s="26"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="32"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="44"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="36"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="48"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="44"/>
-      <c r="C14" s="37" t="s">
+      <c r="B14" s="51"/>
+      <c r="C14" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="36"/>
+      <c r="D14" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="48"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="44"/>
-      <c r="C15" s="37" t="s">
+      <c r="B15" s="51"/>
+      <c r="C15" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="48"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="44"/>
-      <c r="C16" s="37" t="s">
+      <c r="B16" s="51"/>
+      <c r="C16" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="48"/>
     </row>
     <row r="17" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="45"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="42"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="49"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30" t="s">
+      <c r="C18" s="26"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="47"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="44"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="36"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="48"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="44"/>
-      <c r="C20" s="37" t="s">
+      <c r="B20" s="51"/>
+      <c r="C20" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="36"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="48"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="44"/>
-      <c r="C21" s="37" t="s">
+      <c r="B21" s="51"/>
+      <c r="C21" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="36"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="48"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="44"/>
-      <c r="C22" s="37" t="s">
+      <c r="B22" s="51"/>
+      <c r="C22" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="36"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="48"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="44"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="36"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="48"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="44"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="36"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="48"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="44"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="36"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="48"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="44"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="36"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="48"/>
     </row>
     <row r="27" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="45"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="42"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Finished model based section
Completed model based section
</commit_message>
<xml_diff>
--- a/Lit_Review_Tables.xlsx
+++ b/Lit_Review_Tables.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>Method</t>
   </si>
@@ -252,6 +252,21 @@
   <si>
     <t>Large time commitment required for each and every implementation
 Difficult to transfer lessons learned to new applications</t>
+  </si>
+  <si>
+    <t>A Kalman filter may be created for each defined fault state in order to predict the outputs of the compressed air system, and if the prediction error of any filter is zero the system can be diagnosed as being in the relevant fault state</t>
+  </si>
+  <si>
+    <t>Using observers to form hypothesises as to how to change a model to remove deviations from expected behaviour in ordert to diagnose potential faults</t>
+  </si>
+  <si>
+    <t>Manipulating system variables to generate fault signatures in the form of residual differences which can be used in operation to diagnose faults</t>
+  </si>
+  <si>
+    <t>Creating a reference fault-free model of a system and analysing actual deviations in variables to diagnose faults, or tuning model in order to optimise the system with respect to some defined factor (e.g. cost)</t>
+  </si>
+  <si>
+    <t>Formalising potential faults through the use of IF statements to determine when a system is in fault condition by virtue of fundamental engineering principles being broken or changed</t>
   </si>
 </sst>
 </file>
@@ -796,66 +811,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -863,6 +818,66 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1232,7 +1247,7 @@
       </c>
     </row>
     <row r="3" spans="3:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="43" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="14" t="s">
@@ -1246,7 +1261,7 @@
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="3:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="C4" s="39"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1258,7 +1273,7 @@
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="3:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="C5" s="39"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="10" t="s">
         <v>14</v>
       </c>
@@ -1271,7 +1286,7 @@
       <c r="J5" s="20"/>
     </row>
     <row r="6" spans="3:12" ht="45.75" x14ac:dyDescent="0.3">
-      <c r="C6" s="39"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1284,7 +1299,7 @@
       <c r="L6" s="15"/>
     </row>
     <row r="7" spans="3:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="C7" s="39"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
@@ -1298,7 +1313,7 @@
       </c>
     </row>
     <row r="8" spans="3:12" ht="90.75" x14ac:dyDescent="0.3">
-      <c r="C8" s="39"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1311,7 +1326,7 @@
       <c r="J8" s="16"/>
     </row>
     <row r="9" spans="3:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="C9" s="39"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1323,7 +1338,7 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="3:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="C10" s="39"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="10" t="s">
         <v>30</v>
       </c>
@@ -1334,7 +1349,7 @@
       <c r="H10" s="11"/>
     </row>
     <row r="11" spans="3:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="C11" s="40"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1648,8 +1663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1685,199 +1700,209 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="55" t="s">
         <v>44</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="28"/>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="55" t="s">
+      <c r="G3" s="60" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="51"/>
+      <c r="B4" s="56"/>
       <c r="C4" s="34" t="s">
         <v>47</v>
       </c>
       <c r="D4" s="29"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="56"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="61"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="51"/>
+      <c r="B5" s="56"/>
       <c r="C5" s="35" t="s">
         <v>48</v>
       </c>
       <c r="D5" s="30"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="56"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="61"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="51"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="35" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="30"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="56"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="61"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="51"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="35" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="30"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="56"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="61"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="51"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="36" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="31"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="56"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="61"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="51"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="36" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="31"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="56"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="61"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="51"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="36" t="s">
         <v>49</v>
       </c>
       <c r="D10" s="31"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="56"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="61"/>
     </row>
     <row r="11" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="52"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="37" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="32"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="57"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="62"/>
     </row>
     <row r="12" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="60" t="s">
+      <c r="E12" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="60" t="s">
+      <c r="F12" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="61" t="s">
+      <c r="G12" s="41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="51" t="s">
+    <row r="13" spans="2:7" ht="132" x14ac:dyDescent="0.3">
+      <c r="B13" s="56" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="53" t="s">
+      <c r="D13" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="45"/>
-      <c r="G13" s="48"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="51"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="53"/>
+    </row>
+    <row r="14" spans="2:7" ht="99" x14ac:dyDescent="0.3">
+      <c r="B14" s="56"/>
       <c r="C14" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="48"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="51"/>
-      <c r="C15" s="62" t="s">
+      <c r="D14" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="47"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="53"/>
+    </row>
+    <row r="15" spans="2:7" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B15" s="56"/>
+      <c r="C15" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="48"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="51"/>
+      <c r="D15" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="47"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="53"/>
+    </row>
+    <row r="16" spans="2:7" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="56"/>
       <c r="C16" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="48"/>
-    </row>
-    <row r="17" spans="2:7" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="52"/>
+      <c r="D16" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="47"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="53"/>
+    </row>
+    <row r="17" spans="2:7" ht="116.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="57"/>
       <c r="C17" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="49"/>
+      <c r="D17" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="48"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="54"/>
     </row>
     <row r="18" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="60" t="s">
+      <c r="E18" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="G18" s="61" t="s">
+      <c r="G18" s="41" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="55" t="s">
         <v>56</v>
       </c>
       <c r="C19" s="33" t="s">
@@ -1886,107 +1911,107 @@
       <c r="D19" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="41" t="s">
+      <c r="E19" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="44"/>
-      <c r="G19" s="47"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="52"/>
     </row>
     <row r="20" spans="2:7" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B20" s="51"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="35" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="48"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="53"/>
     </row>
     <row r="21" spans="2:7" ht="66" x14ac:dyDescent="0.3">
-      <c r="B21" s="51"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="48"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="53"/>
     </row>
     <row r="22" spans="2:7" ht="66" x14ac:dyDescent="0.3">
-      <c r="B22" s="51"/>
+      <c r="B22" s="56"/>
       <c r="C22" s="35" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="42"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="48"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="53"/>
     </row>
     <row r="23" spans="2:7" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="B23" s="51"/>
+      <c r="B23" s="56"/>
       <c r="C23" s="35" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="48"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="53"/>
     </row>
     <row r="24" spans="2:7" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="B24" s="51"/>
+      <c r="B24" s="56"/>
       <c r="C24" s="35" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="48"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="53"/>
     </row>
     <row r="25" spans="2:7" ht="132" x14ac:dyDescent="0.3">
-      <c r="B25" s="51"/>
+      <c r="B25" s="56"/>
       <c r="C25" s="35" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="42"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="48"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="53"/>
     </row>
     <row r="26" spans="2:7" ht="132" x14ac:dyDescent="0.3">
-      <c r="B26" s="51"/>
+      <c r="B26" s="56"/>
       <c r="C26" s="35" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="48"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="53"/>
     </row>
     <row r="27" spans="2:7" ht="132.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="52"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="37" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="43"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="49"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>